<commit_message>
Bug in validation for LegalType
</commit_message>
<xml_diff>
--- a/files/GDPR setup data.xlsx
+++ b/files/GDPR setup data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel.borge/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB74B537-E653-F745-8E88-E6A096911299}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BCEB4C-4239-634D-823A-80A28B77FA2C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4458,13 +4458,13 @@
           <x14:formula1>
             <xm:f>System!$A$3:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F8:F573</xm:sqref>
+          <xm:sqref>F301:F573</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select valid legal ground" xr:uid="{898966D5-C02E-0942-BD98-41F1AA4A2AE7}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F480E288-021D-9842-996A-0ED0C84D6166}">
           <x14:formula1>
-            <xm:f>'/Users/axel.borge/Documents/[Demo Sesam GDPR setup data .xlsx]System'!#REF!</xm:f>
+            <xm:f>System!$A$3:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F6</xm:sqref>
+          <xm:sqref>F4:F300</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4480,7 +4480,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7346,7 +7346,7 @@
           <x14:formula1>
             <xm:f>System!$C$3:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E294</xm:sqref>
+          <xm:sqref>E3:E300</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Title to Name and Duy to Support
</commit_message>
<xml_diff>
--- a/files/GDPR setup data.xlsx
+++ b/files/GDPR setup data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel.borge/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BCEB4C-4239-634D-823A-80A28B77FA2C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6754ED54-A62C-FD46-8F71-791CEF15DFFF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,16 +17,12 @@
     <sheet name="Data type" sheetId="2" r:id="rId2"/>
     <sheet name="System" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data type'!$A$2:$KR$291</definedName>
     <definedName name="DataTypeID">'Data type'!$A$3:$A$291</definedName>
     <definedName name="PurposeID">Purpose!$A$4:$A$297</definedName>
   </definedNames>
   <calcPr calcId="171026" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,7 +50,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support:</t>
         </r>
         <r>
           <rPr>
@@ -87,7 +83,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -121,7 +127,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -140,43 +156,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>A short name describing the the purpose at a more detailed level than </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>BusinessProcess</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>, for example if the </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>BusinessProcess</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> is "Employment", it can be "Salary" or "Payroll". It is used as a property heading/label in the end-user interface.
+          <t xml:space="preserve">A short name describing the the purpose at a more detailed level than BusinessProcess, for example if the BusinessProcess is "Employment", it can be "Salary" or "Payroll". It is used as a property heading/label in the end-user interface.
 </t>
         </r>
       </text>
@@ -191,7 +171,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -225,7 +215,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -279,7 +279,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -382,7 +392,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -426,7 +446,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -460,7 +490,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -494,7 +534,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -527,7 +577,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -560,7 +620,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -604,7 +674,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -637,7 +717,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -671,7 +761,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -705,7 +805,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -739,7 +849,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -773,7 +893,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Duy Dinh-Steffensen:</t>
+          <t>Sesam-support</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
@@ -909,9 +1039,6 @@
     <t>Personal</t>
   </si>
   <si>
-    <t>duy.dinh-steffensen@sesam.io</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -967,9 +1094,6 @@
   </si>
   <si>
     <t>BusinessProcess</t>
-  </si>
-  <si>
-    <t>Title</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -1039,6 +1163,12 @@
   </si>
   <si>
     <t>PURPOSE</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>support@sesam.io</t>
   </si>
 </sst>
 </file>
@@ -2162,23 +2292,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Purpose"/>
-      <sheetName val="Data type"/>
-      <sheetName val="System"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2442,7 +2555,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y299"/>
+  <dimension ref="A1:Y300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -2468,7 +2581,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2500,10 +2613,10 @@
     <row r="2" spans="1:25" ht="221" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -2511,13 +2624,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>2</v>
@@ -2526,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>4</v>
@@ -2538,126 +2651,132 @@
         <v>6</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="str">
-        <f>LOWER(IF(B4="","",B4 &amp; "-") &amp; IF(F4="","",F4 &amp; "-" ) &amp; SUBSTITUTE(C4," ","_") )</f>
+        <f t="shared" ref="A4:A67" si="0">SUBSTITUTE(LOWER(IF(B4="","",B4 &amp; "-") &amp; IF(F4="","",F4 &amp; "-" ) &amp; C4)," ","_" )</f>
         <v>marketing-consent-email</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
         <v>45</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="str">
-        <f t="shared" ref="A5:A6" si="0">LOWER(IF(B5="","",B5 &amp; "-") &amp; IF(F5="","",F5 &amp; "-" ) &amp; SUBSTITUTE(C5," ","_") )</f>
+        <f t="shared" si="0"/>
         <v>customers-contract-communication</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I5">
         <v>90</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>event-contract-attendee</v>
+        <f>SUBSTITUTE(LOWER(IF(B6="","",B6 &amp; "-") &amp; IF(F6="","",F6 &amp; "-" ) &amp; C6)," ","_" )</f>
+        <v>event-legal_obligation-attendee</v>
       </c>
       <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I6">
         <v>60</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="str">
-        <f t="shared" ref="A8:A67" si="1">LOWER(IF(B8="","",B8 &amp; "-") &amp; IF(F8="","",F8 &amp; "-" ) &amp; SUBSTITUTE(C8," ","_") )</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D8" s="13"/>
@@ -2667,7 +2786,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D9" s="13"/>
@@ -2677,7 +2796,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D10" s="13"/>
@@ -2687,7 +2806,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D11" s="13"/>
@@ -2697,7 +2816,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D12" s="13"/>
@@ -2707,7 +2826,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D13" s="13"/>
@@ -2717,7 +2836,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D14" s="13"/>
@@ -2727,7 +2846,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D15" s="13"/>
@@ -2737,7 +2856,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D16" s="13"/>
@@ -2747,1699 +2866,1705 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="str">
-        <f t="shared" ref="A68:A131" si="2">LOWER(IF(B68="","",B68 &amp; "-") &amp; IF(F68="","",F68 &amp; "-" ) &amp; SUBSTITUTE(C68," ","_") )</f>
+        <f t="shared" ref="A68:A131" si="1">SUBSTITUTE(LOWER(IF(B68="","",B68 &amp; "-") &amp; IF(F68="","",F68 &amp; "-" ) &amp; C68)," ","_" )</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="16" t="str">
-        <f t="shared" ref="A132:A195" si="3">LOWER(IF(B132="","",B132 &amp; "-") &amp; IF(F132="","",F132 &amp; "-" ) &amp; SUBSTITUTE(C132," ","_") )</f>
+        <f t="shared" ref="A132:A195" si="2">SUBSTITUTE(LOWER(IF(B132="","",B132 &amp; "-") &amp; IF(F132="","",F132 &amp; "-" ) &amp; C132)," ","_" )</f>
         <v/>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="16" t="str">
-        <f t="shared" ref="A196:A259" si="4">LOWER(IF(B196="","",B196 &amp; "-") &amp; IF(F196="","",F196 &amp; "-" ) &amp; SUBSTITUTE(C196," ","_") )</f>
+        <f t="shared" ref="A196:A259" si="3">SUBSTITUTE(LOWER(IF(B196="","",B196 &amp; "-") &amp; IF(F196="","",F196 &amp; "-" ) &amp; C196)," ","_" )</f>
         <v/>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="16" t="str">
-        <f t="shared" ref="A260:A299" si="5">LOWER(IF(B260="","",B260 &amp; "-") &amp; IF(F260="","",F260 &amp; "-" ) &amp; SUBSTITUTE(C260," ","_") )</f>
+        <f t="shared" ref="A260:A300" si="4">SUBSTITUTE(LOWER(IF(B260="","",B260 &amp; "-") &amp; IF(F260="","",F260 &amp; "-" ) &amp; C260)," ","_" )</f>
         <v/>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="16" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -4480,7 +4605,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4599,7 +4724,7 @@
         <v>customers-contract-communication</v>
       </c>
       <c r="J2" s="3" t="str">
-        <v>event-contract-attendee</v>
+        <v>event-legal_obligation-attendee</v>
       </c>
       <c r="K2" s="3" t="str">
         <v/>
@@ -5500,7 +5625,7 @@
         <v>salesforce-task</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -5510,16 +5635,16 @@
         <v>Task from Salesforce</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:314" x14ac:dyDescent="0.2">
@@ -5528,7 +5653,7 @@
         <v>salesforce-lead</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -5541,13 +5666,13 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:314" x14ac:dyDescent="0.2">
@@ -5556,7 +5681,7 @@
         <v>salesforce-eventrelation</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -5566,16 +5691,16 @@
         <v>Eventrelation from Salesforce</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:314" x14ac:dyDescent="0.2">
@@ -5597,16 +5722,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:314" x14ac:dyDescent="0.2">
@@ -7332,13 +7457,11 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="F4:F6" r:id="rId3" display="support@sesam.io" xr:uid="{C9D3D259-4DAA-8A45-9ACA-66C3C2888C0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -7370,12 +7493,12 @@
   <sheetData>
     <row r="1" spans="1:26" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
       <c r="D1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -7402,11 +7525,11 @@
     </row>
     <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -7419,35 +7542,35 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document 32 char limit in type ids
</commit_message>
<xml_diff>
--- a/files/GDPR setup data.xlsx
+++ b/files/GDPR setup data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel.borge/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\lake\python\lake\docs\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6754ED54-A62C-FD46-8F71-791CEF15DFFF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A17B4E-9CBF-424B-822C-CFE474288DBB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="DataTypeID">'Data type'!$A$3:$A$291</definedName>
     <definedName name="PurposeID">Purpose!$A$4:$A$297</definedName>
   </definedNames>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -674,17 +674,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sesam-support</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>:</t>
+          <t>Sesam-support:</t>
         </r>
         <r>
           <rPr>
@@ -703,7 +693,28 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The ID of the data type - it is automatically computed from the other columns. </t>
+          <t xml:space="preserve">The ID of the data type - it is automatically computed from the other columns. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note that it must be less than 32 characters long. Please limit "System" and/or "Type" size accordingly.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -849,17 +860,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sesam-support</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>:</t>
+          <t>Sesam-support:</t>
         </r>
         <r>
           <rPr>
@@ -878,7 +879,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The "level" of the data - it can be either "Personal" or "Related", i.e. directly about the data subject or indirectly (for example data about the customer such as address or orders for the customer, respectively)
+          <t xml:space="preserve">The "level" of the data - it can be either "Personal" or "Related", i.e. directly about the data subject or indirectly (for example data about the customer such as address or orders for the customer, respectively). You should have at least one "Personal" level row.
 </t>
         </r>
       </text>
@@ -893,17 +894,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sesam-support</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>:</t>
+          <t>Sesam-support:</t>
         </r>
         <r>
           <rPr>
@@ -922,8 +913,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">An comma separated list of email-addresses for who should get notified when a GDPR data access request or change request is received by the GDPR platform.
-</t>
+          <t>An comma separated list of email-addresses for who should get notified when a GDPR data access request or change request is received by the GDPR platform. There should not be any whitespace before or after the comma.</t>
         </r>
       </text>
     </comment>
@@ -1175,7 +1165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1354,6 +1344,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2561,10 +2558,10 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.83203125" style="12" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -2579,7 +2576,7 @@
     <col min="12" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="52" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
@@ -2610,7 +2607,7 @@
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
     </row>
-    <row r="2" spans="1:25" ht="221" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="221" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
         <v>33</v>
@@ -2619,7 +2616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="20" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -2657,7 +2654,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="str">
         <f t="shared" ref="A4:A67" si="0">SUBSTITUTE(LOWER(IF(B4="","",B4 &amp; "-") &amp; IF(F4="","",F4 &amp; "-" ) &amp; C4)," ","_" )</f>
         <v>marketing-consent-email</v>
@@ -2694,7 +2691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="str">
         <f t="shared" si="0"/>
         <v>customers-contract-communication</v>
@@ -2731,7 +2728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="str">
         <f>SUBSTITUTE(LOWER(IF(B6="","",B6 &amp; "-") &amp; IF(F6="","",F6 &amp; "-" ) &amp; C6)," ","_" )</f>
         <v>event-legal_obligation-attendee</v>
@@ -2768,13 +2765,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2784,7 +2781,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2794,7 +2791,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2804,7 +2801,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2814,7 +2811,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2824,7 +2821,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2834,7 +2831,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2844,7 +2841,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2854,7 +2851,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2864,1705 +2861,1705 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="str">
         <f t="shared" ref="A68:A131" si="1">SUBSTITUTE(LOWER(IF(B68="","",B68 &amp; "-") &amp; IF(F68="","",F68 &amp; "-" ) &amp; C68)," ","_" )</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="16" t="str">
         <f t="shared" ref="A132:A195" si="2">SUBSTITUTE(LOWER(IF(B132="","",B132 &amp; "-") &amp; IF(F132="","",F132 &amp; "-" ) &amp; C132)," ","_" )</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" s="16" t="str">
         <f t="shared" ref="A196:A259" si="3">SUBSTITUTE(LOWER(IF(B196="","",B196 &amp; "-") &amp; IF(F196="","",F196 &amp; "-" ) &amp; C196)," ","_" )</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260" s="16" t="str">
         <f t="shared" ref="A260:A300" si="4">SUBSTITUTE(LOWER(IF(B260="","",B260 &amp; "-") &amp; IF(F260="","",F260 &amp; "-" ) &amp; C260)," ","_" )</f>
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A265" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A267" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A281" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A288" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A289" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A290" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A291" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A292" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A293" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A294" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A295" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A296" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A297" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A298" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A299" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A300" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4605,10 +4602,10 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -4622,7 +4619,7 @@
     <col min="10" max="10" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:314" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:314" ht="56" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -4696,7 +4693,7 @@
       <c r="BO1" s="7"/>
       <c r="BP1" s="7"/>
     </row>
-    <row r="2" spans="1:314" s="2" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:314" s="2" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -5619,7 +5616,7 @@
       <c r="LA2" s="3"/>
       <c r="LB2" s="3"/>
     </row>
-    <row r="3" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A58" si="0">SUBSTITUTE(LOWER(IF(C3="","",C3 &amp;"-" ) &amp; B3)," ","_")</f>
         <v>salesforce-task</v>
@@ -5647,7 +5644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>salesforce-lead</v>
@@ -5675,7 +5672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>salesforce-eventrelation</v>
@@ -5703,7 +5700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>salesforce-contact</v>
@@ -5734,1715 +5731,1715 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:314" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:314" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="str">
         <f t="shared" ref="A59:A122" si="2">SUBSTITUTE(LOWER(IF(C59="","",C59 &amp;"-" ) &amp; B59)," ","_")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="str">
         <f t="shared" ref="A123:A186" si="3">SUBSTITUTE(LOWER(IF(C123="","",C123 &amp;"-" ) &amp; B123)," ","_")</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="str">
         <f t="shared" ref="A187:A250" si="4">SUBSTITUTE(LOWER(IF(C187="","",C187 &amp;"-" ) &amp; B187)," ","_")</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="str">
         <f t="shared" ref="A251:A291" si="5">SUBSTITUTE(LOWER(IF(C251="","",C251 &amp;"-" ) &amp; B251)," ","_")</f>
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A281" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A288" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A291" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -7485,13 +7482,13 @@
       <selection activeCell="A3" sqref="A3:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="52" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -7523,7 +7520,7 @@
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
     </row>
-    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>24</v>
       </c>
@@ -7532,7 +7529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -7540,7 +7537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -7548,27 +7545,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>

</xml_diff>